<commit_message>
testing a values of a row
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -30,13 +30,13 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Krishna Sapktoa</t>
-  </si>
-  <si>
     <t>303 Hollow Way</t>
   </si>
   <si>
     <t>ks_21285@hotmail.com</t>
+  </si>
+  <si>
+    <t>Krishna Sapkota</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A5:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,16 +413,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
       </c>
       <c r="C6">
         <v>7727682394</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test for setting values in excel
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Krishna Sapkota</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -386,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:D6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,6 +403,14 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>

</xml_diff>